<commit_message>
tumorboards clean und vom 29.06.2025 im RAO Ordner
</commit_message>
<xml_diff>
--- a/tumorboards/Neuro/alle_tumorboards_neuro.xlsx
+++ b/tumorboards/Neuro/alle_tumorboards_neuro.xlsx
@@ -2,21 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14145" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="30_06_2025" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,11 +48,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -415,30 +418,1433 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Sammel-Excel für Tumorboard: Neuro-Onkologie</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Erstellt automatisch durch USZ-RAO-App</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jeder Tab repräsentiert ein Tumorboard-Datum</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L23"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="35" customWidth="1" min="9" max="9"/>
+    <col width="21" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Sammel-Excel für Tumorboard: Neuro-Onkologie</t>
+          <t>Patientennummer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Geschlecht</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Geburtsdatum</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Diagnose</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ICD-10</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Beschreibung ICD-10</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Radiotherapie indiziert</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Art des Aufgebots</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Teams Priorisierung</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Vormerken für Studie</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Bemerkung/Procedere</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Erstellt automatisch durch USZ-RAO-App</t>
+      <c r="A2" t="n">
+        <v>11427434</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ammann Lorenz</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>08.05.1965</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Glioblastom im Gyrus frontalis medius rechts, WHO Grad 4, IDH-Wildtyp, ED 27.01.2025</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>C71.2</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung: Temporallappen</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Kat I: In 1-3 Tagen ohne Konsil</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Guckenberger</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nicht qualifiziert</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>dawds</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Jeder Tab repräsentiert ein Tumorboard-Datum</t>
+      <c r="A3" t="n">
+        <v>10943154</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bernasconi Corinne</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>13.07.1994</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pleomorphes Xanthoastrozytom, WHO Grad 3, temporal rechts, ED 26.09.2020</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>C71.2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Temporallappens</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Kat II: In 5-7 Tagen ohne Konsil</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Linsenmeier</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nicht qualifiziert</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10272440</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bonomi Andrea Giuseppe</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>25.03.1965</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Incidental right precentral meningeal mass 17 x 6 mm, probably meningioma, ED 2014</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>D32.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung der Hirnhäute des Gehirns</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Kat III: Nach Eingang des Konsils</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Guninski</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CHESS</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>dasdaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>11454161</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bühler Margrith</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>18.02.1942</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Meningeom ausgehend von inferiorer duraler Begrenzung des Sinus cavernosus links, ED 2025</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>D32.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung der Hirnhäute des Gehirns</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>11455875</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dauti Rini</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>03.02.1974</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Myxopapilläres Ependymom, WHO Grad 2, höhe L1/2 links ED 04/25</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>D33.4</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung des Rückenmarkes</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10506896</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>de Zilva Priscilla Pearl Constance</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>19.10.1979</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>41- jährige Patientin mit sekundär metastasiertem (cerebral), duktalem Mammakarzinom links, initial: pT2,</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>C79.3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sekundäre bösartige Neubildung des Gehirns und der Hirnhäute</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>11349604</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ehrler Alois Martin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>05.05.1954</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Glioblastom im Gyrus frontalis superior, IDH-Wildtyp, MGMT eher methyliert, CNS WHO Grad 4, ED</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>C71.1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Frontallappens</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>60232951</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Fleischli Denise</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>09.01.1987</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Schubförmige Multiple Sklerose, ES ca. 2008, ED 04/2019, EDSS 3.0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>G35</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Multiple Sklerose</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11457978</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Gentner Veronika</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>20532</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Zerebral und pulmonal metastasiertes Adenokarzinom des rechten Unterlappens, ED 28.04.2025</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>C79.3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Sekundäre bösartige Neubildung des Gehirns und der Hirnhäute</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3412148</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Gutmann Rupert</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>20676</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Multiple intrakranielle Meningeome, St.n. mehrfachen Resektionen und Bestrahlungen, zuletzt Resektion eines parasagittalen Meningeoms rechts frontal WHO Grad 3 08/2024</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>C70.0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung der Meningen des Gehirns</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10009296</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Hoffmann Volker</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>23134</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Glioblastom parietookzipital rechts IDH Wildtyp, CNS WHO Grad 4, ED 06.02.2025</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>C71.8</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Gehirns, mehrere Teilbereiche überlappend</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10653445</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hösli Fiona Elena</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>04.12.1997</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Intrauterin diagnostizierter Hydrocephalus occlusivus bei zystischer Raumforderung mit Verlegung des</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>G91.1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Obstruktiver Hydrozephalus</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4249593</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Iten Jürg</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>22226</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Glioblastom, WHO Grad 4, Gyrus supramarginalis rechts, ED 19.07.2024</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>C71.3</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bösartige Neubildung des Parietallappens </t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10645326</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jost Urs</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>14.04.1958</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ioblastom links parietal, WHO Grad 4, MGMT-Promoter methyliert, ED 02/2024</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>C71.3</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Parietallappens</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2835720</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Kamm Margrit</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>03.07.1942</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Meningeom parieto-okzipital links, ED 28.03.2025</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>D32.0</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung der Hirnhäute des Gehirns</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>7487762</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Krasniqi Elbatrit</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>34466</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Neu diagnostizierte intraaxiale wenig KM-affine Raumforderung temporal rechts, ED 20.06.2025</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>D43.0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Neubildung unsicheren oder unbekannten Verhaltens des Gehirns, supratentoriell</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>11471643</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Lanfranchi Guido Angelo</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>25.06.1959</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Multiple metastasenverdächtige Raumforderungen cerebral, ED 10.06.2025</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>C79.3</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Sekundäre bösartige Neubildung des Gehirns und der Hirnhäute</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10356428</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Müller Andrea Helena Maria</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>23.11.1972</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Oligodendrogliom, WHO-Grad 2, operkulär links, ED 11/2016</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>C71.9</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Gehirns, nicht näher bezeichnet</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>11410212</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Nevoigt Jürgen Peter</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>21.07.1970</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Postoperativ liquorgefüllte Zyste rechts cerebellär i.R. Diagnose 2, ED 01.02.2025</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>G93.0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Zerebrale Zysten</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3758834</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Oechslin Rosmarie</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12.07.1954</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Glioblastom, IDH-Wildtyp CNS WHO-Grad 4, im Cuneus links, ED 12.03.2023</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>C71.4</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Bösartige Neubildung des Okzipitallappens</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>11459603</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Plüss Susanna</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>21.04.1955</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Keilbeinflügelmeningeom links, ED 25.01.2024</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>D32.0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung der Hirnhäute des Gehirns</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>10397448</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Roth Martha</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>14004</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Atypisches Meningeom (WHO Grad II) postcentral</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>D32.0</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Gutartige Neubildung der Meningen: Hirnhäute</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>